<commit_message>
cambio en la primera rama del arpa
subiendo el commit en la rama 1 de arpa
</commit_message>
<xml_diff>
--- a/arp -a.xlsx
+++ b/arp -a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Documents\kraken\offic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F7A32DE-119F-4C09-9A9F-2CE8F479CBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E536166-E252-49A0-8288-7F83A4B1FF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14226ABE-A5E2-497F-B7A9-199C2B2C3592}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="741">
   <si>
     <t>169.254.29.113        18-3d-2d-4c-03-31     dinámico</t>
   </si>
@@ -2262,6 +2262,9 @@
   </si>
   <si>
     <t>arp -a</t>
+  </si>
+  <si>
+    <t>en la rama 1,</t>
   </si>
 </sst>
 </file>
@@ -2759,10 +2762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7CEBC7-F76B-445C-A052-55231E07A4B8}">
-  <dimension ref="A1:G281"/>
+  <dimension ref="A1:K281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,189 +2778,192 @@
     <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <f>MID(A2,1,14)</f>
         <v>169.254.29.113</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2" s="1" t="str">
         <f>MID(A2,22,20)</f>
         <v xml:space="preserve"> 18-3d-2d-4c-03-31  </v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <f t="shared" ref="C3:C66" si="0">MID(A3,1,14)</f>
         <v xml:space="preserve">  192.168.3.1 </v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <f t="shared" ref="D3:D66" si="1">MID(A3,22,20)</f>
         <v xml:space="preserve">   08-3a-88-19-1f-97</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.3 </v>
       </c>
-      <c r="D4" t="str">
+      <c r="D4" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   dc-4e-f4-2e-10-2a</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="K4" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.4 </v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   88-ae-dd-07-ba-1e</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.5 </v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   b0-cc-fe-92-00-9a</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.7 </v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   94-de-80-2f-37-ed</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.8 </v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   1c-66-6d-92-99-89</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.9 </v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   cc-28-aa-33-17-18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.10</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   38-60-77-8a-93-9e</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
2do cambio en la rama 1 de arpa
commit del 2do cambio en la rama 2 de arpa
</commit_message>
<xml_diff>
--- a/arp -a.xlsx
+++ b/arp -a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Documents\kraken\offic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E536166-E252-49A0-8288-7F83A4B1FF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D7A36D-0A80-4E91-A87E-CE051CF3BCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14226ABE-A5E2-497F-B7A9-199C2B2C3592}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="742">
   <si>
     <t>169.254.29.113        18-3d-2d-4c-03-31     dinámico</t>
   </si>
@@ -2265,6 +2265,9 @@
   </si>
   <si>
     <t>en la rama 1,</t>
+  </si>
+  <si>
+    <t>en la rama 1</t>
   </si>
 </sst>
 </file>
@@ -2305,7 +2308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2333,6 +2336,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2365,7 +2380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2427,6 +2442,8 @@
     <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2765,7 +2782,7 @@
   <dimension ref="A1:K281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,387 +2980,393 @@
         <v>493</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.11</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   28-87-ba-42-53-fb</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="27" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.12</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   dc-4e-f4-2d-fb-a8</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="27" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.13</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   e0-d5-5e-57-c0-84</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="27" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.14</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   dc-4e-f4-2e-42-26</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="27" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.15</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   90-2b-34-13-f0-00</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="27" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.16</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   18-3d-2d-4c-00-98</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="27" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="K16" s="27" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.17</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   00-71-c2-3e-7a-8f</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="27" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.18</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   18-3d-2d-4c-00-f6</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="27" t="s">
         <v>465</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="27" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.19</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   74-fe-ce-6e-66-0b</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="27" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.20</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20" s="27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   e4-11-5b-bc-c0-22</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="27" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.21</v>
       </c>
-      <c r="D21" t="str">
+      <c r="D21" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   1c-1b-0d-c8-87-d0</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="28" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C22" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.22</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D22" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   cc-28-aa-33-06-e0</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="28" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.23</v>
       </c>
-      <c r="D23" t="str">
+      <c r="D23" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   00-e0-4d-a9-5c-e2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="28" t="s">
         <v>472</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="28" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C24" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.25</v>
       </c>
-      <c r="D24" t="str">
+      <c r="D24" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   18-3d-2d-4c-00-63</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="28" t="s">
         <v>473</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="28" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.26</v>
       </c>
-      <c r="D25" t="str">
+      <c r="D25" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   9c-b6-54-bb-6f-94</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="28" t="s">
         <v>474</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="28" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="K25" s="28" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.27</v>
       </c>
-      <c r="D26" t="str">
+      <c r="D26" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   cc-28-aa-33-38-52</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="28" t="s">
         <v>475</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="28" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.28</v>
       </c>
-      <c r="D27" t="str">
+      <c r="D27" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   00-e0-4c-68-0a-e0</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="28" t="s">
         <v>476</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="28" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.29</v>
       </c>
-      <c r="D28" t="str">
+      <c r="D28" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   cc-28-aa-32-f0-42</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="28" t="s">
         <v>477</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="28" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.30</v>
       </c>
-      <c r="D29" t="str">
+      <c r="D29" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   4c-cc-6a-7b-98-69</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="28" t="s">
         <v>478</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="28" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.31</v>
       </c>
-      <c r="D30" t="str">
+      <c r="D30" s="28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">   40-8d-5c-80-c6-f2</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="28" t="s">
         <v>479</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="28" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3362,7 +3385,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
kitando fondo de color a una columna de enmedio al arp y commitiando
</commit_message>
<xml_diff>
--- a/arp -a.xlsx
+++ b/arp -a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Documents\kraken\offic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D7A36D-0A80-4E91-A87E-CE051CF3BCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0FCA37-20FA-4083-9A73-387177FC884A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14226ABE-A5E2-497F-B7A9-199C2B2C3592}"/>
+    <workbookView xWindow="1020" yWindow="450" windowWidth="26985" windowHeight="14715" xr2:uid="{14226ABE-A5E2-497F-B7A9-199C2B2C3592}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2380,7 +2380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2444,6 +2444,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2782,7 +2783,7 @@
   <dimension ref="A1:K281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,6 +2800,7 @@
       <c r="A1" s="1" t="s">
         <v>739</v>
       </c>
+      <c r="C1" s="29"/>
       <c r="F1" s="1" t="s">
         <v>483</v>
       </c>
@@ -2810,7 +2812,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="C2" s="29" t="str">
         <f>MID(A2,1,14)</f>
         <v>169.254.29.113</v>
       </c>
@@ -2829,7 +2831,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="str">
+      <c r="C3" s="29" t="str">
         <f t="shared" ref="C3:C66" si="0">MID(A3,1,14)</f>
         <v xml:space="preserve">  192.168.3.1 </v>
       </c>
@@ -2848,7 +2850,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.3 </v>
       </c>
@@ -2870,7 +2872,7 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.4 </v>
       </c>
@@ -2889,7 +2891,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C6" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.5 </v>
       </c>
@@ -2908,7 +2910,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.7 </v>
       </c>
@@ -2927,7 +2929,7 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C8" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.8 </v>
       </c>
@@ -2946,7 +2948,7 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C9" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.9 </v>
       </c>
@@ -2965,7 +2967,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C10" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.10</v>
       </c>
@@ -2984,7 +2986,7 @@
       <c r="A11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="27" t="str">
+      <c r="C11" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.11</v>
       </c>
@@ -3003,7 +3005,7 @@
       <c r="A12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="27" t="str">
+      <c r="C12" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.12</v>
       </c>
@@ -3022,7 +3024,7 @@
       <c r="A13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="27" t="str">
+      <c r="C13" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.13</v>
       </c>
@@ -3041,7 +3043,7 @@
       <c r="A14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="27" t="str">
+      <c r="C14" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.14</v>
       </c>
@@ -3060,7 +3062,7 @@
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="27" t="str">
+      <c r="C15" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.15</v>
       </c>
@@ -3079,7 +3081,7 @@
       <c r="A16" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="27" t="str">
+      <c r="C16" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.16</v>
       </c>
@@ -3101,7 +3103,7 @@
       <c r="A17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="27" t="str">
+      <c r="C17" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.17</v>
       </c>
@@ -3120,7 +3122,7 @@
       <c r="A18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="27" t="str">
+      <c r="C18" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.18</v>
       </c>
@@ -3139,7 +3141,7 @@
       <c r="A19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="27" t="str">
+      <c r="C19" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.19</v>
       </c>
@@ -3158,7 +3160,7 @@
       <c r="A20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="27" t="str">
+      <c r="C20" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.20</v>
       </c>
@@ -3177,7 +3179,7 @@
       <c r="A21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="28" t="str">
+      <c r="C21" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.21</v>
       </c>
@@ -3196,7 +3198,7 @@
       <c r="A22" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="28" t="str">
+      <c r="C22" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.22</v>
       </c>
@@ -3215,7 +3217,7 @@
       <c r="A23" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="28" t="str">
+      <c r="C23" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.23</v>
       </c>
@@ -3234,7 +3236,7 @@
       <c r="A24" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="28" t="str">
+      <c r="C24" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.25</v>
       </c>
@@ -3253,7 +3255,7 @@
       <c r="A25" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="28" t="str">
+      <c r="C25" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.26</v>
       </c>
@@ -3275,7 +3277,7 @@
       <c r="A26" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="28" t="str">
+      <c r="C26" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.27</v>
       </c>
@@ -3294,7 +3296,7 @@
       <c r="A27" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="28" t="str">
+      <c r="C27" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.28</v>
       </c>
@@ -3313,7 +3315,7 @@
       <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="28" t="str">
+      <c r="C28" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.29</v>
       </c>
@@ -3332,7 +3334,7 @@
       <c r="A29" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="28" t="str">
+      <c r="C29" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.30</v>
       </c>
@@ -3351,7 +3353,7 @@
       <c r="A30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="28" t="str">
+      <c r="C30" s="29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  192.168.3.31</v>
       </c>

</xml_diff>